<commit_message>
fichier excel formation et site
</commit_message>
<xml_diff>
--- a/Ressources/site_import.xlsx
+++ b/Ressources/site_import.xlsx
@@ -621,14 +621,14 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" customWidth="1"/>
     <col min="5" max="5" width="41.28515625" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" customWidth="1"/>
@@ -639,10 +639,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -656,10 +656,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -673,10 +673,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -690,10 +690,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>11</v>
@@ -706,11 +706,11 @@
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5">
         <v>94000</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>14</v>
@@ -724,10 +724,10 @@
         <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -741,10 +741,10 @@
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>20</v>
@@ -758,10 +758,10 @@
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>23</v>
@@ -775,10 +775,10 @@
         <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>26</v>
@@ -792,10 +792,10 @@
         <v>30</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>29</v>
@@ -809,10 +809,10 @@
         <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>32</v>
@@ -826,10 +826,10 @@
         <v>36</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>35</v>
@@ -843,10 +843,10 @@
         <v>39</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>38</v>
@@ -860,10 +860,10 @@
         <v>42</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>41</v>
@@ -877,10 +877,10 @@
         <v>45</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>44</v>
@@ -894,10 +894,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>47</v>
@@ -911,10 +911,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>49</v>
@@ -928,10 +928,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>51</v>
@@ -945,10 +945,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>53</v>
@@ -962,10 +962,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>55</v>
@@ -978,11 +978,11 @@
       <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="5">
         <v>94400</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>57</v>

</xml_diff>